<commit_message>
Add base bus routing (#4)
</commit_message>
<xml_diff>
--- a/data/bus_stops.xlsx
+++ b/data/bus_stops.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huilunang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huilunang/Desktop/Projects/SIT-UOG/2022_2023_TRI2/SIT_AY22-23_CSC1108/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8F535F-A517-E649-ACC6-957DAC077860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36FF144-C4D4-BD40-8A01-733E35456F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="500" windowWidth="23180" windowHeight="16300" activeTab="7" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
+    <workbookView xWindow="5620" yWindow="500" windowWidth="23180" windowHeight="16300" xr2:uid="{F10A9419-1CB3-714B-AE05-C7B58E3111EF}"/>
   </bookViews>
   <sheets>
     <sheet name="P101-loop" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>1.4627466510403129, 103.73965194475493</t>
   </si>
   <si>
-    <t>Maktab Sultan Abu Bakar (English College</t>
-  </si>
-  <si>
     <t>Hospital Sultanah Aminah</t>
   </si>
   <si>
@@ -1089,6 +1086,9 @@
   </si>
   <si>
     <t>Taman Mewah</t>
+  </si>
+  <si>
+    <t>Maktab Sultan Abu Bakar (English College)</t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B383786-A1E5-0A42-A2B9-65DCA6F0CA76}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1454,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1512,10 +1512,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,7 +1523,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>343</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1534,10 +1534,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,10 +1545,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,10 +1556,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,10 +1567,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1578,10 +1578,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,10 +1589,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1600,10 +1600,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,10 +1611,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1622,10 +1622,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1633,10 +1633,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1644,10 +1644,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,10 +1655,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1666,7 +1666,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1694,7 +1694,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1708,10 +1708,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1719,10 +1719,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1730,10 +1730,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1741,10 +1741,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1752,10 +1752,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1763,10 +1763,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1774,10 +1774,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1785,10 +1785,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1796,10 +1796,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1807,10 +1807,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1818,10 +1818,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1829,10 +1829,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1840,10 +1840,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1851,10 +1851,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1862,10 +1862,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1873,10 +1873,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1884,10 +1884,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1895,10 +1895,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1906,10 +1906,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1917,10 +1917,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1928,10 +1928,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1939,10 +1939,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1950,10 +1950,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1961,10 +1961,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -1989,7 +1989,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2003,10 +2003,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2014,10 +2014,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2025,10 +2025,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2036,10 +2036,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2047,10 +2047,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2058,10 +2058,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2069,10 +2069,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,10 +2080,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2091,10 +2091,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2119,7 +2119,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2133,10 +2133,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2144,10 +2144,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,10 +2155,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2166,10 +2166,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2177,10 +2177,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2188,10 +2188,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2199,10 +2199,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2210,10 +2210,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2221,10 +2221,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2232,10 +2232,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2243,10 +2243,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2254,10 +2254,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2282,7 +2282,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2296,10 +2296,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2307,10 +2307,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2318,10 +2318,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2329,10 +2329,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2340,10 +2340,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2351,10 +2351,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2362,10 +2362,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2373,10 +2373,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,10 +2384,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2395,10 +2395,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2406,10 +2406,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2417,10 +2417,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2428,10 +2428,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2439,10 +2439,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2450,10 +2450,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2461,10 +2461,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2472,10 +2472,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2483,10 +2483,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2494,10 +2494,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,10 +2505,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2516,10 +2516,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2527,10 +2527,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2538,10 +2538,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2549,10 +2549,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2560,10 +2560,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2571,10 +2571,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2582,10 +2582,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2593,10 +2593,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2604,10 +2604,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2615,10 +2615,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2626,10 +2626,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2637,10 +2637,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2648,10 +2648,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2659,10 +2659,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2687,7 +2687,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2701,10 +2701,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2712,10 +2712,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2723,10 +2723,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2734,10 +2734,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2745,10 +2745,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2756,10 +2756,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
         <v>139</v>
-      </c>
-      <c r="C7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2767,10 +2767,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2778,10 +2778,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2789,10 +2789,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2800,10 +2800,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2811,10 +2811,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2822,10 +2822,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2833,10 +2833,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2844,10 +2844,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2855,10 +2855,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2866,10 +2866,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2877,10 +2877,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2888,10 +2888,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2899,10 +2899,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2910,10 +2910,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2921,10 +2921,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2932,10 +2932,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2943,10 +2943,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2954,10 +2954,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2965,10 +2965,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2976,10 +2976,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2987,10 +2987,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2998,10 +2998,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3009,10 +3009,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3020,10 +3020,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3048,7 +3048,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3062,10 +3062,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3073,10 +3073,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3084,10 +3084,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3095,10 +3095,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3106,10 +3106,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3117,10 +3117,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3128,10 +3128,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3139,10 +3139,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3150,10 +3150,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3161,10 +3161,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3172,10 +3172,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3183,10 +3183,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3194,10 +3194,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" t="s">
         <v>206</v>
-      </c>
-      <c r="C14" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3205,10 +3205,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3216,10 +3216,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3227,10 +3227,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3238,10 +3238,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3249,10 +3249,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3260,10 +3260,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3271,10 +3271,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3282,10 +3282,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3293,10 +3293,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" t="s">
         <v>224</v>
-      </c>
-      <c r="C23" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3304,10 +3304,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3315,10 +3315,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3326,10 +3326,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3337,7 +3337,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -3365,7 +3365,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3379,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3393,7 +3393,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3401,10 +3401,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3412,10 +3412,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3423,10 +3423,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3434,10 +3434,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3445,10 +3445,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3456,10 +3456,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3467,10 +3467,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3478,10 +3478,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3489,10 +3489,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3500,10 +3500,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3511,10 +3511,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3522,10 +3522,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3533,10 +3533,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3544,10 +3544,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3555,10 +3555,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3566,10 +3566,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3577,10 +3577,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3588,10 +3588,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3599,10 +3599,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3610,10 +3610,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3621,10 +3621,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3632,10 +3632,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3643,10 +3643,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3654,10 +3654,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3665,10 +3665,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3676,10 +3676,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3692,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09611D23-CBEC-BB47-8C1C-593243700395}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3704,7 +3704,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3718,10 +3718,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3729,10 +3729,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3740,10 +3740,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3751,10 +3751,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3762,10 +3762,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3773,10 +3773,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3784,10 +3784,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3795,10 +3795,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3806,10 +3806,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3817,10 +3817,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3828,10 +3828,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3839,10 +3839,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3850,10 +3850,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3861,10 +3861,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3872,10 +3872,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3883,10 +3883,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3894,10 +3894,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,10 +3905,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" t="s">
         <v>206</v>
-      </c>
-      <c r="C19" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3916,10 +3916,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3927,10 +3927,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3938,10 +3938,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3949,10 +3949,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3960,10 +3960,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3971,10 +3971,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3982,10 +3982,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3993,10 +3993,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4004,10 +4004,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" t="s">
         <v>224</v>
-      </c>
-      <c r="C28" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -4015,10 +4015,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4026,10 +4026,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -4037,10 +4037,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4048,7 +4048,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -4076,7 +4076,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4090,7 +4090,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -4104,7 +4104,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4112,10 +4112,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4123,10 +4123,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4134,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -4145,10 +4145,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4156,10 +4156,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4167,10 +4167,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4178,10 +4178,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4189,10 +4189,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4200,10 +4200,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -4211,10 +4211,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -4222,10 +4222,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -4233,10 +4233,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -4244,10 +4244,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4255,10 +4255,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4266,10 +4266,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4277,10 +4277,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -4288,10 +4288,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4299,10 +4299,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4310,10 +4310,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4321,10 +4321,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4332,10 +4332,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4343,10 +4343,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4354,10 +4354,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4365,10 +4365,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4376,10 +4376,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -4387,10 +4387,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4398,10 +4398,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -4409,10 +4409,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4420,10 +4420,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -4431,10 +4431,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -4442,10 +4442,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C34" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -4453,10 +4453,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -4464,10 +4464,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>